<commit_message>
schedule funcionando con daemon
</commit_message>
<xml_diff>
--- a/data/Matriz_de_adyacencia_data_team.xlsx
+++ b/data/Matriz_de_adyacencia_data_team.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diani\Dropbox\1 TESIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaronga\Documents\GitHub\data-engineering\pipelines\dagster\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC2D9E4-00E1-40C4-8CAD-4885B247E882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC66980-ACCE-47B3-AF28-25AFF6F47826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz de adyacencia" sheetId="1" r:id="rId1"/>
@@ -753,10 +753,10 @@
   <dimension ref="A1:AZ52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AH7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="AY30" sqref="AY30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3762,58 +3762,156 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0</v>
+      </c>
+      <c r="L20" s="3">
+        <v>1</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0</v>
+      </c>
+      <c r="N20" s="3">
+        <v>0</v>
+      </c>
+      <c r="O20" s="3">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0</v>
+      </c>
+      <c r="R20" s="3">
+        <v>1</v>
+      </c>
+      <c r="S20" s="3">
+        <v>1</v>
+      </c>
       <c r="T20" s="15">
         <v>0</v>
       </c>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
-      <c r="AF20" s="3"/>
-      <c r="AG20" s="3"/>
-      <c r="AH20" s="3"/>
-      <c r="AI20" s="3"/>
-      <c r="AJ20" s="3"/>
-      <c r="AK20" s="3"/>
-      <c r="AL20" s="3"/>
-      <c r="AM20" s="3"/>
-      <c r="AN20" s="3"/>
-      <c r="AO20" s="3"/>
-      <c r="AP20" s="3"/>
-      <c r="AQ20" s="3"/>
-      <c r="AR20" s="3"/>
-      <c r="AS20" s="3"/>
-      <c r="AT20" s="3"/>
-      <c r="AU20" s="3"/>
-      <c r="AV20" s="3"/>
-      <c r="AW20" s="3"/>
-      <c r="AX20" s="3"/>
-      <c r="AY20" s="3"/>
-      <c r="AZ20" s="3"/>
+      <c r="U20" s="3">
+        <v>0</v>
+      </c>
+      <c r="V20" s="3">
+        <v>1</v>
+      </c>
+      <c r="W20" s="8">
+        <v>0</v>
+      </c>
+      <c r="X20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AX20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AZ20" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -3822,58 +3920,156 @@
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
+        <v>1</v>
+      </c>
+      <c r="L21" s="3">
+        <v>1</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0</v>
+      </c>
+      <c r="N21" s="3">
+        <v>0</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0</v>
+      </c>
+      <c r="R21" s="3">
+        <v>1</v>
+      </c>
+      <c r="S21" s="3">
+        <v>0</v>
+      </c>
+      <c r="T21" s="3">
+        <v>1</v>
+      </c>
       <c r="U21" s="15">
         <v>0</v>
       </c>
-      <c r="V21" s="3"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
-      <c r="AA21" s="3"/>
-      <c r="AB21" s="3"/>
-      <c r="AC21" s="3"/>
-      <c r="AD21" s="3"/>
-      <c r="AE21" s="3"/>
-      <c r="AF21" s="3"/>
-      <c r="AG21" s="3"/>
-      <c r="AH21" s="3"/>
-      <c r="AI21" s="3"/>
-      <c r="AJ21" s="3"/>
-      <c r="AK21" s="3"/>
-      <c r="AL21" s="3"/>
-      <c r="AM21" s="3"/>
-      <c r="AN21" s="3"/>
-      <c r="AO21" s="3"/>
-      <c r="AP21" s="3"/>
-      <c r="AQ21" s="3"/>
-      <c r="AR21" s="3"/>
-      <c r="AS21" s="3"/>
-      <c r="AT21" s="3"/>
-      <c r="AU21" s="3"/>
-      <c r="AV21" s="3"/>
-      <c r="AW21" s="3"/>
-      <c r="AX21" s="3"/>
-      <c r="AY21" s="3"/>
-      <c r="AZ21" s="3"/>
+      <c r="V21" s="3">
+        <v>0</v>
+      </c>
+      <c r="W21" s="8">
+        <v>1</v>
+      </c>
+      <c r="X21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AP21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AX21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AZ21" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -3882,58 +4078,156 @@
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3">
+        <v>1</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3">
+        <v>1</v>
+      </c>
+      <c r="M22" s="3">
+        <v>1</v>
+      </c>
+      <c r="N22" s="3">
+        <v>1</v>
+      </c>
+      <c r="O22" s="3">
+        <v>1</v>
+      </c>
+      <c r="P22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>0</v>
+      </c>
+      <c r="R22" s="3">
+        <v>0</v>
+      </c>
+      <c r="S22" s="3">
+        <v>0</v>
+      </c>
+      <c r="T22" s="3">
+        <v>0</v>
+      </c>
+      <c r="U22" s="3">
+        <v>0</v>
+      </c>
       <c r="V22" s="15">
         <v>0</v>
       </c>
-      <c r="W22" s="8"/>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="3"/>
-      <c r="AB22" s="3"/>
-      <c r="AC22" s="3"/>
-      <c r="AD22" s="3"/>
-      <c r="AE22" s="3"/>
-      <c r="AF22" s="3"/>
-      <c r="AG22" s="3"/>
-      <c r="AH22" s="3"/>
-      <c r="AI22" s="3"/>
-      <c r="AJ22" s="3"/>
-      <c r="AK22" s="3"/>
-      <c r="AL22" s="3"/>
-      <c r="AM22" s="3"/>
-      <c r="AN22" s="3"/>
-      <c r="AO22" s="3"/>
-      <c r="AP22" s="3"/>
-      <c r="AQ22" s="3"/>
-      <c r="AR22" s="3"/>
-      <c r="AS22" s="3"/>
-      <c r="AT22" s="3"/>
-      <c r="AU22" s="3"/>
-      <c r="AV22" s="3"/>
-      <c r="AW22" s="3"/>
-      <c r="AX22" s="3"/>
-      <c r="AY22" s="3"/>
-      <c r="AZ22" s="3"/>
+      <c r="W22" s="3">
+        <v>0</v>
+      </c>
+      <c r="X22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AH22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AJ22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AL22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AM22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AN22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AO22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AP22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AW22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AX22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AZ22" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
@@ -3942,58 +4236,156 @@
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
+      <c r="C23" s="3">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0</v>
+      </c>
+      <c r="N23" s="3">
+        <v>0</v>
+      </c>
+      <c r="O23" s="3">
+        <v>0</v>
+      </c>
+      <c r="P23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>0</v>
+      </c>
+      <c r="R23" s="3">
+        <v>0</v>
+      </c>
+      <c r="S23" s="3">
+        <v>0</v>
+      </c>
+      <c r="T23" s="3">
+        <v>0</v>
+      </c>
+      <c r="U23" s="3">
+        <v>0</v>
+      </c>
+      <c r="V23" s="3">
+        <v>0</v>
+      </c>
       <c r="W23" s="15">
-        <v>0</v>
-      </c>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-      <c r="Z23" s="3"/>
-      <c r="AA23" s="3"/>
-      <c r="AB23" s="3"/>
-      <c r="AC23" s="3"/>
-      <c r="AD23" s="3"/>
-      <c r="AE23" s="3"/>
-      <c r="AF23" s="3"/>
-      <c r="AG23" s="3"/>
-      <c r="AH23" s="3"/>
-      <c r="AI23" s="3"/>
-      <c r="AJ23" s="3"/>
-      <c r="AK23" s="3"/>
-      <c r="AL23" s="3"/>
-      <c r="AM23" s="3"/>
-      <c r="AN23" s="3"/>
-      <c r="AO23" s="3"/>
-      <c r="AP23" s="3"/>
-      <c r="AQ23" s="3"/>
-      <c r="AR23" s="3"/>
-      <c r="AS23" s="3"/>
-      <c r="AT23" s="3"/>
-      <c r="AU23" s="3"/>
-      <c r="AV23" s="3"/>
-      <c r="AW23" s="3"/>
-      <c r="AX23" s="3"/>
-      <c r="AY23" s="3"/>
-      <c r="AZ23" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="X23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AP23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV23" s="3">
+        <v>1</v>
+      </c>
+      <c r="AW23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AX23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AY23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AZ23" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A24" s="4">

</xml_diff>